<commit_message>
Add add sub-activity to visual (ctd)
</commit_message>
<xml_diff>
--- a/plan_visual_django/tests/resources/input_files/excel_plan_files_not_unit/NewFSProduct-PlanForPlan.xlsx
+++ b/plan_visual_django/tests/resources/input_files/excel_plan_files_not_unit/NewFSProduct-PlanForPlan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Development/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Development/PycharmProjects/plan_visualiser2025/plan_visual_django/tests/resources/input_files/excel_plan_files_not_unit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E686C4F8-94D4-B543-B8BA-48558CE49D27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33BE0F3E-9BC7-9E41-8387-D4A2B31E79D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4180" yWindow="500" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -511,7 +511,7 @@
     <t>Target End Of Discovery</t>
   </si>
   <si>
-    <t>Task_Name</t>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -863,7 +863,7 @@
   <dimension ref="A1:O59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>